<commit_message>
Re-running MSI and updating all output files
</commit_message>
<xml_diff>
--- a/out/table_comparison.xlsx
+++ b/out/table_comparison.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee02903/Documents/Research Projects/Github/PSY8960- Class Projects/psy8960-week11/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26734BE6-9429-5744-9496-0C8FAAD32831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9828AD-45A0-A84C-8BE8-D6FE3D30DDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="500" windowWidth="13740" windowHeight="15520" xr2:uid="{5374FEA6-3FF0-4D40-A0F0-EE88B41B675A}"/>
+    <workbookView xWindow="1060" yWindow="1200" windowWidth="13740" windowHeight="15460" xr2:uid="{5374FEA6-3FF0-4D40-A0F0-EE88B41B675A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,13 +457,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
@@ -480,7 +480,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -493,18 +493,18 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>8.6679999999999993</v>
+        <v>8.6739999999999995</v>
       </c>
       <c r="G3">
-        <v>7.97199999999998</v>
+        <v>6.1929999999999801</v>
       </c>
       <c r="H3">
         <f>(G3-F3)/F3</f>
-        <v>-8.0295339178590136E-2</v>
+        <v>-0.28602720774729301</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -517,18 +517,18 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>17.696000000000002</v>
+        <v>17.846</v>
       </c>
       <c r="G4">
-        <v>3.9780000000000002</v>
+        <v>3.1840000000000201</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H13" si="0">(G4-F4)/F4</f>
-        <v>-0.77520343580470163</v>
+        <v>-0.82158466883335091</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
@@ -541,18 +541,18 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>49.423000000000002</v>
+        <v>46.921999999999997</v>
       </c>
       <c r="G5">
-        <v>32.857999999999997</v>
+        <v>32.091000000000001</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>-0.33516783683710022</v>
+        <v>-0.31607774604663053</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
@@ -565,14 +565,14 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <v>220.048</v>
+        <v>220.60599999999999</v>
       </c>
       <c r="G6">
-        <v>21.634</v>
+        <v>19.498999999999999</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>-0.90168508689013305</v>
+        <v>-0.91161165154166257</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating response for MSI output and comparison file
</commit_message>
<xml_diff>
--- a/out/table_comparison.xlsx
+++ b/out/table_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lee02903/Documents/Research Projects/Github/PSY8960- Class Projects/psy8960-week11/out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9828AD-45A0-A84C-8BE8-D6FE3D30DDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B359090C-7AE8-C34C-8675-8097D960E15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1200" windowWidth="13740" windowHeight="15460" xr2:uid="{5374FEA6-3FF0-4D40-A0F0-EE88B41B675A}"/>
+    <workbookView xWindow="18800" yWindow="0" windowWidth="10000" windowHeight="18000" xr2:uid="{5374FEA6-3FF0-4D40-A0F0-EE88B41B675A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,14 +614,14 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>2.97</v>
+        <v>3.28</v>
       </c>
       <c r="G10">
-        <v>3.11</v>
+        <v>3.04</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>4.7138047138047028E-2</v>
+        <v>-7.3170731707317013E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,14 +638,14 @@
         <v>4</v>
       </c>
       <c r="F11">
-        <v>5.78</v>
+        <v>5.95</v>
       </c>
       <c r="G11">
         <v>1.91</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>-0.66955017301038067</v>
+        <v>-0.67899159663865549</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -662,14 +662,14 @@
         <v>5</v>
       </c>
       <c r="F12">
-        <v>36.5</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="G12">
-        <v>35.4</v>
+        <v>34.6</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>-3.0136986301369902E-2</v>
+        <v>-8.4656084656084554E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -686,14 +686,14 @@
         <v>6</v>
       </c>
       <c r="F13">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G13">
         <v>28</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>-0.78125</v>
+        <v>-0.78294573643410847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>